<commit_message>
state of project after turning in IS490DB final project
</commit_message>
<xml_diff>
--- a/Database Design/FinalProjectTablePlanV2.xlsx
+++ b/Database Design/FinalProjectTablePlanV2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenna/Documents/GitHub/international-relations-database/Database Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{032ABAD9-384A-9E42-BF68-F8B3CEB45FE4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DA5262-FBA7-774F-B7FB-5CAC9786EBE2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16400" yWindow="460" windowWidth="12300" windowHeight="16120" xr2:uid="{075452CA-2087-9849-A48A-F3F6DE116604}"/>
+    <workbookView xWindow="15900" yWindow="460" windowWidth="12800" windowHeight="16120" xr2:uid="{075452CA-2087-9849-A48A-F3F6DE116604}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="105">
   <si>
     <t>Table Name</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Primary Key</t>
   </si>
   <si>
-    <t>varchar2</t>
-  </si>
-  <si>
     <t>candidate key</t>
   </si>
   <si>
@@ -82,12 +79,6 @@
     <t>EndDate</t>
   </si>
   <si>
-    <t>integer</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>STATE_DATES</t>
   </si>
   <si>
@@ -184,9 +175,6 @@
     <t>WarID</t>
   </si>
   <si>
-    <t>WarName</t>
-  </si>
-  <si>
     <t>WarType</t>
   </si>
   <si>
@@ -238,9 +226,6 @@
     <t>igoID</t>
   </si>
   <si>
-    <t>igoAbbreviation</t>
-  </si>
-  <si>
     <t>igoShortName</t>
   </si>
   <si>
@@ -292,9 +277,6 @@
     <t>STATE_RESOURCE</t>
   </si>
   <si>
-    <t>Resource</t>
-  </si>
-  <si>
     <t>Amount</t>
   </si>
   <si>
@@ -319,13 +301,46 @@
     <t>ToWar</t>
   </si>
   <si>
-    <t>TransitionID</t>
-  </si>
-  <si>
-    <t>Foreign Key to WAR.WarID</t>
-  </si>
-  <si>
     <t>WAR_TRANSITIONS</t>
+  </si>
+  <si>
+    <t>NUMBER</t>
+  </si>
+  <si>
+    <t>VARCHAR2</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>igoAbbr</t>
+  </si>
+  <si>
+    <t>WarShortName</t>
+  </si>
+  <si>
+    <t>WarLongName</t>
+  </si>
+  <si>
+    <t>WarTypeName</t>
+  </si>
+  <si>
+    <t>IN(1, 2, 3, 4, 5)</t>
+  </si>
+  <si>
+    <t>IN(1, 2, 3, 4, 5, 6)</t>
+  </si>
+  <si>
+    <t>IN(0, 1)</t>
+  </si>
+  <si>
+    <t>ResourceID</t>
+  </si>
+  <si>
+    <t>AllianceType</t>
+  </si>
+  <si>
+    <t>IN (0, 1)</t>
   </si>
 </sst>
 </file>
@@ -361,8 +376,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,17 +693,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C52A4E9F-50A3-3745-B725-E73FA28118F3}">
-  <dimension ref="A1:D116"/>
+  <dimension ref="A1:D119"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.83203125" customWidth="1"/>
     <col min="2" max="2" width="17.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -698,7 +714,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -712,8 +728,8 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>18</v>
+      <c r="C2" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -724,13 +740,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -738,35 +754,35 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
-        <v>18</v>
+      <c r="C5" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
@@ -774,118 +790,118 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
         <v>21</v>
       </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" t="s">
-        <v>18</v>
+      <c r="C15" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
@@ -893,90 +909,93 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" t="s">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" t="s">
-        <v>18</v>
+        <v>24</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" t="s">
-        <v>7</v>
+        <v>23</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" t="s">
-        <v>18</v>
+        <v>29</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
@@ -984,24 +1003,24 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" t="s">
-        <v>7</v>
+        <v>43</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" t="s">
-        <v>18</v>
+        <v>40</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
@@ -1009,234 +1028,264 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" t="s">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D27" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" t="s">
-        <v>18</v>
+        <v>26</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D28" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" t="s">
-        <v>19</v>
+        <v>28</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" t="s">
-        <v>18</v>
+        <v>22</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" t="s">
-        <v>18</v>
+        <v>34</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" t="s">
-        <v>18</v>
+        <v>29</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D33" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" t="s">
-        <v>18</v>
+        <v>31</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" t="s">
-        <v>18</v>
+        <v>30</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
-      </c>
-      <c r="C36" t="s">
-        <v>18</v>
+        <v>37</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
-      </c>
-      <c r="C37" t="s">
-        <v>18</v>
+        <v>38</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
-      </c>
-      <c r="C38" t="s">
-        <v>18</v>
+        <v>44</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39" t="s">
-        <v>18</v>
+        <v>32</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" t="s">
-        <v>18</v>
+        <v>33</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" t="s">
-        <v>18</v>
+        <v>35</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D41" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
-      </c>
-      <c r="C42" t="s">
-        <v>18</v>
+        <v>36</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D42" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B43" t="s">
-        <v>48</v>
-      </c>
-      <c r="C43" t="s">
-        <v>18</v>
+        <v>45</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B44" t="s">
-        <v>49</v>
-      </c>
-      <c r="C44" t="s">
-        <v>18</v>
+        <v>46</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B45" t="s">
         <v>5</v>
       </c>
-      <c r="C45" t="s">
-        <v>18</v>
+      <c r="C45" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D45" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B46" t="s">
-        <v>25</v>
-      </c>
-      <c r="C46" t="s">
-        <v>18</v>
+        <v>22</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D46" t="s">
         <v>6</v>
@@ -1244,13 +1293,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B47" t="s">
-        <v>88</v>
-      </c>
-      <c r="C47" t="s">
-        <v>7</v>
+        <v>102</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="D47" t="s">
         <v>6</v>
@@ -1258,68 +1307,68 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B48" t="s">
-        <v>89</v>
-      </c>
-      <c r="C48" t="s">
-        <v>18</v>
+        <v>83</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B49" t="s">
-        <v>90</v>
-      </c>
-      <c r="C49" t="s">
-        <v>7</v>
+        <v>84</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B50" t="s">
-        <v>91</v>
-      </c>
-      <c r="C50" t="s">
-        <v>7</v>
+        <v>85</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B51" t="s">
-        <v>92</v>
-      </c>
-      <c r="C51" t="s">
-        <v>7</v>
+        <v>86</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>82</v>
+      </c>
+      <c r="B52" t="s">
         <v>87</v>
       </c>
-      <c r="B52" t="s">
-        <v>93</v>
-      </c>
-      <c r="C52" t="s">
-        <v>7</v>
+      <c r="C52" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B53" t="s">
-        <v>69</v>
-      </c>
-      <c r="C53" t="s">
-        <v>18</v>
+        <v>65</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D53" t="s">
         <v>6</v>
@@ -1327,121 +1376,121 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B54" t="s">
-        <v>70</v>
-      </c>
-      <c r="C54" t="s">
-        <v>7</v>
+        <v>95</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="D54" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B55" t="s">
-        <v>71</v>
-      </c>
-      <c r="C55" t="s">
-        <v>7</v>
+        <v>66</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B56" t="s">
-        <v>72</v>
-      </c>
-      <c r="C56" t="s">
-        <v>7</v>
+        <v>67</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B57" t="s">
-        <v>12</v>
-      </c>
-      <c r="C57" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>15</v>
-      </c>
-      <c r="C58" t="s">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" t="s">
         <v>68</v>
       </c>
-      <c r="B59" t="s">
-        <v>73</v>
-      </c>
-      <c r="C59" t="s">
-        <v>7</v>
+      <c r="C59" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B60" t="s">
-        <v>26</v>
-      </c>
-      <c r="C60" t="s">
-        <v>7</v>
+        <v>23</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B61" t="s">
-        <v>69</v>
-      </c>
-      <c r="C61" t="s">
-        <v>18</v>
+        <v>65</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D61" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B62" t="s">
         <v>5</v>
       </c>
-      <c r="C62" t="s">
-        <v>18</v>
+      <c r="C62" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D62" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B63" t="s">
-        <v>76</v>
-      </c>
-      <c r="C63" t="s">
-        <v>18</v>
+        <v>71</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D63" t="s">
         <v>6</v>
@@ -1449,24 +1498,24 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B64" t="s">
-        <v>77</v>
-      </c>
-      <c r="C64" t="s">
-        <v>18</v>
+        <v>72</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B65" t="s">
-        <v>80</v>
-      </c>
-      <c r="C65" t="s">
-        <v>18</v>
+        <v>75</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D65" t="s">
         <v>6</v>
@@ -1474,140 +1523,140 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B66" t="s">
-        <v>27</v>
-      </c>
-      <c r="C66" t="s">
-        <v>7</v>
+        <v>103</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B67" t="s">
-        <v>16</v>
-      </c>
-      <c r="C67" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B68" t="s">
-        <v>17</v>
-      </c>
-      <c r="C68" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B69" t="s">
-        <v>12</v>
-      </c>
-      <c r="C69" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B70" t="s">
-        <v>11</v>
-      </c>
-      <c r="C70" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B71" t="s">
-        <v>10</v>
-      </c>
-      <c r="C71" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B72" t="s">
-        <v>15</v>
-      </c>
-      <c r="C72" t="s">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B73" t="s">
-        <v>14</v>
-      </c>
-      <c r="C73" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>13</v>
-      </c>
-      <c r="C74" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>80</v>
-      </c>
-      <c r="C75" t="s">
-        <v>18</v>
+        <v>75</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D75" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B76" t="s">
         <v>5</v>
       </c>
-      <c r="C76" t="s">
-        <v>18</v>
+      <c r="C76" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D76" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>16</v>
-      </c>
-      <c r="C77" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="D77" t="s">
         <v>6</v>
@@ -1615,146 +1664,146 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>17</v>
-      </c>
-      <c r="C78" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B79" t="s">
-        <v>12</v>
-      </c>
-      <c r="C79" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B80" t="s">
-        <v>11</v>
-      </c>
-      <c r="C80" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B81" t="s">
-        <v>10</v>
-      </c>
-      <c r="C81" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B82" t="s">
-        <v>15</v>
-      </c>
-      <c r="C82" t="s">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B83" t="s">
-        <v>14</v>
-      </c>
-      <c r="C83" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B84" t="s">
-        <v>13</v>
-      </c>
-      <c r="C84" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B85" t="s">
-        <v>80</v>
-      </c>
-      <c r="C85" t="s">
-        <v>18</v>
+        <v>75</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D85" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B86" t="s">
         <v>5</v>
       </c>
-      <c r="C86" t="s">
-        <v>18</v>
+      <c r="C86" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D86" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B87" t="s">
-        <v>16</v>
-      </c>
-      <c r="C87" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="D87" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B88" t="s">
-        <v>85</v>
-      </c>
-      <c r="C88" t="s">
-        <v>7</v>
+        <v>80</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="D88" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B89" t="s">
-        <v>51</v>
-      </c>
-      <c r="C89" t="s">
-        <v>18</v>
+        <v>48</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D89" t="s">
         <v>6</v>
@@ -1762,124 +1811,121 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B90" t="s">
-        <v>52</v>
-      </c>
-      <c r="C90" t="s">
-        <v>7</v>
+        <v>96</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B91" t="s">
-        <v>53</v>
-      </c>
-      <c r="C91" t="s">
-        <v>18</v>
+        <v>97</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B92" t="s">
-        <v>64</v>
-      </c>
-      <c r="C92" t="s">
-        <v>18</v>
+        <v>49</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B93" t="s">
-        <v>59</v>
-      </c>
-      <c r="C93" t="s">
-        <v>18</v>
+        <v>98</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B94" t="s">
-        <v>60</v>
-      </c>
-      <c r="C94" t="s">
-        <v>18</v>
+        <v>55</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B95" t="s">
-        <v>51</v>
-      </c>
-      <c r="C95" t="s">
-        <v>18</v>
-      </c>
-      <c r="D95" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B96" t="s">
-        <v>56</v>
-      </c>
-      <c r="C96" t="s">
-        <v>7</v>
+        <v>48</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D96" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B97" t="s">
-        <v>51</v>
-      </c>
-      <c r="C97" t="s">
-        <v>18</v>
+        <v>52</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="D97" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B98" t="s">
-        <v>65</v>
-      </c>
-      <c r="C98" t="s">
-        <v>7</v>
+        <v>48</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D98" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B99" t="s">
-        <v>16</v>
-      </c>
-      <c r="C99" t="s">
-        <v>19</v>
+        <v>61</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="D99" t="s">
         <v>6</v>
@@ -1887,207 +1933,249 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B100" t="s">
-        <v>17</v>
-      </c>
-      <c r="C100" t="s">
-        <v>19</v>
+        <v>63</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D100" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B101" t="s">
-        <v>12</v>
-      </c>
-      <c r="C101" t="s">
-        <v>18</v>
+        <v>5</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D101" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B102" t="s">
-        <v>11</v>
-      </c>
-      <c r="C102" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D102" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B103" t="s">
-        <v>10</v>
-      </c>
-      <c r="C103" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B104" t="s">
-        <v>15</v>
-      </c>
-      <c r="C104" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B105" t="s">
-        <v>14</v>
-      </c>
-      <c r="C105" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B106" t="s">
-        <v>13</v>
-      </c>
-      <c r="C106" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B107" t="s">
-        <v>51</v>
-      </c>
-      <c r="C107" t="s">
-        <v>18</v>
-      </c>
-      <c r="D107" t="s">
-        <v>55</v>
+        <v>14</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B108" t="s">
-        <v>65</v>
-      </c>
-      <c r="C108" t="s">
-        <v>7</v>
-      </c>
-      <c r="D108" t="s">
-        <v>6</v>
+        <v>13</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B109" t="s">
-        <v>67</v>
-      </c>
-      <c r="C109" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B110" t="s">
-        <v>5</v>
-      </c>
-      <c r="C110" t="s">
-        <v>18</v>
+        <v>48</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D110" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
+        <v>57</v>
+      </c>
+      <c r="B111" t="s">
         <v>61</v>
       </c>
-      <c r="B111" t="s">
-        <v>62</v>
-      </c>
-      <c r="C111" t="s">
-        <v>7</v>
+      <c r="C111" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D111" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B112" t="s">
-        <v>66</v>
-      </c>
-      <c r="C112" t="s">
-        <v>18</v>
+        <v>63</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D112" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B113" t="s">
-        <v>63</v>
-      </c>
-      <c r="C113" t="s">
-        <v>18</v>
+        <v>5</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D113" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>99</v>
+        <v>57</v>
       </c>
       <c r="B114" t="s">
-        <v>97</v>
-      </c>
-      <c r="C114" t="s">
-        <v>18</v>
-      </c>
-      <c r="D114" t="s">
-        <v>6</v>
+        <v>58</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>99</v>
+        <v>57</v>
       </c>
       <c r="B115" t="s">
-        <v>95</v>
-      </c>
-      <c r="C115" t="s">
-        <v>18</v>
-      </c>
-      <c r="D115" t="s">
-        <v>98</v>
+        <v>62</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>99</v>
+        <v>57</v>
       </c>
       <c r="B116" t="s">
-        <v>96</v>
-      </c>
-      <c r="C116" t="s">
-        <v>18</v>
-      </c>
-      <c r="D116" t="s">
-        <v>98</v>
+        <v>59</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>57</v>
+      </c>
+      <c r="B117" t="s">
+        <v>60</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>91</v>
+      </c>
+      <c r="B118" t="s">
+        <v>89</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D118" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>91</v>
+      </c>
+      <c r="B119" t="s">
+        <v>90</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D119" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>